<commit_message>
Reran the script and added a tool to simplify the concanentated attributes and some other functionality
</commit_message>
<xml_diff>
--- a/DemoMapsAndFiles/MAPA_conversions.xlsx
+++ b/DemoMapsAndFiles/MAPA_conversions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\igswzcwwgsrio\loco\Team\Crow\_Python\MapMerger\DemoMaps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\igswzcwwgsrio\loco\Team\Crow\_Python\MapMerger\DemoMapsAndFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF38C01-2BD5-46FA-8342-F11134260423}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A958AC4B-71F6-4C38-9620-7691089ACE33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Qfp</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Cz</t>
   </si>
 </sst>
 </file>
@@ -938,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,6 +1006,14 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>